<commit_message>
improved data from analysis
</commit_message>
<xml_diff>
--- a/analise_tempos.xlsx
+++ b/analise_tempos.xlsx
@@ -19,6 +19,8 @@
     <definedName name="csv_10000_1000000.txt.time.txt" localSheetId="0">tempos!$O$14:$X$15</definedName>
     <definedName name="filename" localSheetId="0">tempos!$C$27:$C$29</definedName>
     <definedName name="filename_1" localSheetId="0">tempos!$B$6:$B$17</definedName>
+    <definedName name="filename_2" localSheetId="0">tempos!$E$34:$E$45</definedName>
+    <definedName name="filename_3" localSheetId="0">tempos!$T$35:$T$46</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -707,7 +709,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="31">
   <si>
     <t>0.005</t>
   </si>
@@ -722,6 +724,84 @@
   </si>
   <si>
     <t>media</t>
+  </si>
+  <si>
+    <t>soma</t>
+  </si>
+  <si>
+    <t>Column1</t>
+  </si>
+  <si>
+    <t>Column2</t>
+  </si>
+  <si>
+    <t>Column3</t>
+  </si>
+  <si>
+    <t>Column4</t>
+  </si>
+  <si>
+    <t>Column5</t>
+  </si>
+  <si>
+    <t>Column6</t>
+  </si>
+  <si>
+    <t>Column7</t>
+  </si>
+  <si>
+    <t>Column8</t>
+  </si>
+  <si>
+    <t>Column9</t>
+  </si>
+  <si>
+    <t>Column10</t>
+  </si>
+  <si>
+    <t>Column11</t>
+  </si>
+  <si>
+    <t>Column12</t>
+  </si>
+  <si>
+    <t>Column13</t>
+  </si>
+  <si>
+    <t>Column14</t>
+  </si>
+  <si>
+    <t>Column15</t>
+  </si>
+  <si>
+    <t>Column16</t>
+  </si>
+  <si>
+    <t>Column17</t>
+  </si>
+  <si>
+    <t>Column18</t>
+  </si>
+  <si>
+    <t>Column19</t>
+  </si>
+  <si>
+    <t>Column20</t>
+  </si>
+  <si>
+    <t>Column21</t>
+  </si>
+  <si>
+    <t>Column22</t>
+  </si>
+  <si>
+    <t>Column23</t>
+  </si>
+  <si>
+    <t>Column24</t>
+  </si>
+  <si>
+    <t>Column25</t>
   </si>
 </sst>
 </file>
@@ -773,8 +853,22 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="61">
+  <cellStyleXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -841,7 +935,7 @@
     <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="61">
+  <cellStyles count="75">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -872,6 +966,13 @@
     <cellStyle name="Followed Hyperlink" xfId="56" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="58" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="60" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="62" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="64" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="66" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="68" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="70" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="72" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="74" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -902,47 +1003,401 @@
     <cellStyle name="Hyperlink" xfId="55" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="57" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="59" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="61" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="63" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="65" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="67" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="69" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="71" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="73" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="23">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="164" formatCode="0.000"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
 </styleSheet>
 </file>
 
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="118"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="18"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:trendline>
+            <c:trendlineType val="power"/>
+            <c:dispRSqr val="0"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:layout/>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:cat>
+            <c:numRef>
+              <c:f>Table2[Column1]</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>200.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10000.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>10100.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>20000.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>50000.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>100000.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>200000.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>400000.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.01E6</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.05E6</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>2.2E6</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>5.05E6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>tempos!$AN$34:$AN$46</c:f>
+              <c:numCache>
+                <c:formatCode>0,000</c:formatCode>
+                <c:ptCount val="13"/>
+                <c:pt idx="0">
+                  <c:v>0.0043</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.0056</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.07345</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.0574</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.1386</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.40015</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.7755</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.61645</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>3.1934</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>6.75515</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>8.059350000000001</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>16.67605</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>39.54555</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="-2132669688"/>
+        <c:axId val="-2121726072"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="-2132669688"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2121726072"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2121726072"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines/>
+        <c:numFmt formatCode="0,000" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:crossAx val="-2132669688"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="1.0" l="0.75" r="0.75" t="1.0" header="0.5" footer="0.5"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>279400</xdr:colOff>
+      <xdr:row>50</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>28</xdr:col>
+      <xdr:colOff>469900</xdr:colOff>
+      <xdr:row>64</xdr:row>
+      <xdr:rowOff>165100</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="filename_3" connectionId="12" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable10.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="filename" connectionId="13" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable11.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="comma" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="filename_2" connectionId="12" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+</file>
+
+<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="csv_10000_1000000.txt.time.txt" connectionId="7" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="csv_10000_10000.txt.time.txt" connectionId="6" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="csv_10000_0.txt.time.txt" connectionId="5" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="csv_100_10000.txt.time.txt" connectionId="4" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="csv_100_100.txt.time.txt" connectionId="3" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="csv_100_0.txt.time.txt" connectionId="2" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
 <queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="filename_1" connectionId="12" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
-<file path=xl/queryTables/queryTable8.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="filename" connectionId="13" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
-</file>
-
-<file path=xl/queryTables/queryTable9.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="comma" connectionId="1" autoFormatId="0" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="1" applyPatternFormats="1" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="2" name="Table2" displayName="Table2" ref="P33:AN46" totalsRowShown="0" headerRowDxfId="1">
+  <autoFilter ref="P33:AN46"/>
+  <sortState ref="P34:AN46">
+    <sortCondition ref="P33:P46"/>
+  </sortState>
+  <tableColumns count="25">
+    <tableColumn id="1" name="Column1" dataDxfId="0">
+      <calculatedColumnFormula>MAX(Q34,Q34+R34)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="2" name="Column2"/>
+    <tableColumn id="3" name="Column3"/>
+    <tableColumn id="4" name="Column4" dataDxfId="22"/>
+    <tableColumn id="5" name="Column5" dataDxfId="21"/>
+    <tableColumn id="6" name="Column6" dataDxfId="20"/>
+    <tableColumn id="7" name="Column7" dataDxfId="19"/>
+    <tableColumn id="8" name="Column8" dataDxfId="18"/>
+    <tableColumn id="9" name="Column9" dataDxfId="17"/>
+    <tableColumn id="10" name="Column10" dataDxfId="16"/>
+    <tableColumn id="11" name="Column11" dataDxfId="15"/>
+    <tableColumn id="12" name="Column12" dataDxfId="14"/>
+    <tableColumn id="13" name="Column13" dataDxfId="13"/>
+    <tableColumn id="14" name="Column14" dataDxfId="12"/>
+    <tableColumn id="15" name="Column15" dataDxfId="11"/>
+    <tableColumn id="16" name="Column16" dataDxfId="10"/>
+    <tableColumn id="17" name="Column17" dataDxfId="9"/>
+    <tableColumn id="18" name="Column18" dataDxfId="8"/>
+    <tableColumn id="19" name="Column19" dataDxfId="7"/>
+    <tableColumn id="20" name="Column20" dataDxfId="6"/>
+    <tableColumn id="21" name="Column21" dataDxfId="5"/>
+    <tableColumn id="22" name="Column22" dataDxfId="4"/>
+    <tableColumn id="23" name="Column23" dataDxfId="3"/>
+    <tableColumn id="24" name="Column24"/>
+    <tableColumn id="25" name="Column25" dataDxfId="2">
+      <calculatedColumnFormula>AVERAGE(S34:AL34)</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1267,10 +1722,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A3:U29"/>
+  <dimension ref="A3:AN56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="A28" sqref="A28"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="S52" sqref="S52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -1278,15 +1733,16 @@
     <col min="1" max="1" width="11.6640625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="6.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="6" width="5.83203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="9" width="7.1640625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.1640625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="6" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.1640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="8.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="7.1640625" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="8.1640625" bestFit="1" customWidth="1"/>
-    <col min="15" max="383" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="16" max="24" width="11" customWidth="1"/>
+    <col min="25" max="40" width="12" customWidth="1"/>
+    <col min="41" max="383" width="5.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="3" spans="1:21">
@@ -1849,7 +2305,7 @@
         <v>40.521000000000001</v>
       </c>
     </row>
-    <row r="17" spans="1:14">
+    <row r="17" spans="1:40">
       <c r="B17" s="2">
         <v>7.1999999999999995E-2</v>
       </c>
@@ -1890,7 +2346,7 @@
         <v>42.136000000000003</v>
       </c>
     </row>
-    <row r="18" spans="1:14">
+    <row r="18" spans="1:40">
       <c r="B18" s="2">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -1931,7 +2387,7 @@
         <v>39.906999999999996</v>
       </c>
     </row>
-    <row r="19" spans="1:14">
+    <row r="19" spans="1:40">
       <c r="B19" s="2">
         <v>7.5999999999999998E-2</v>
       </c>
@@ -1972,7 +2428,7 @@
         <v>38.389000000000003</v>
       </c>
     </row>
-    <row r="20" spans="1:14">
+    <row r="20" spans="1:40">
       <c r="B20" s="2">
         <v>7.3999999999999996E-2</v>
       </c>
@@ -2013,7 +2469,7 @@
         <v>35.938000000000002</v>
       </c>
     </row>
-    <row r="21" spans="1:14">
+    <row r="21" spans="1:40">
       <c r="B21" s="2">
         <v>7.2999999999999995E-2</v>
       </c>
@@ -2054,7 +2510,7 @@
         <v>40.164999999999999</v>
       </c>
     </row>
-    <row r="22" spans="1:14">
+    <row r="22" spans="1:40">
       <c r="B22" s="2">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -2095,7 +2551,7 @@
         <v>40.201999999999998</v>
       </c>
     </row>
-    <row r="23" spans="1:14">
+    <row r="23" spans="1:40">
       <c r="B23" s="2">
         <v>6.9000000000000006E-2</v>
       </c>
@@ -2136,7 +2592,7 @@
         <v>40.042000000000002</v>
       </c>
     </row>
-    <row r="24" spans="1:14">
+    <row r="24" spans="1:40">
       <c r="B24" s="2">
         <v>7.1999999999999995E-2</v>
       </c>
@@ -2177,7 +2633,7 @@
         <v>46.317</v>
       </c>
     </row>
-    <row r="25" spans="1:14">
+    <row r="25" spans="1:40">
       <c r="B25" s="2">
         <v>6.9000000000000006E-2</v>
       </c>
@@ -2218,7 +2674,7 @@
         <v>41.621000000000002</v>
       </c>
     </row>
-    <row r="26" spans="1:14">
+    <row r="26" spans="1:40">
       <c r="B26" s="2">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -2259,7 +2715,7 @@
         <v>37.539000000000001</v>
       </c>
     </row>
-    <row r="28" spans="1:14">
+    <row r="28" spans="1:40">
       <c r="A28" t="s">
         <v>4</v>
       </c>
@@ -2316,12 +2772,2020 @@
         <v>39.545549999999999</v>
       </c>
     </row>
-    <row r="29" spans="1:14">
+    <row r="29" spans="1:40">
       <c r="B29" s="1"/>
+    </row>
+    <row r="32" spans="1:40">
+      <c r="P32" t="s">
+        <v>5</v>
+      </c>
+      <c r="AN32" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="2:40">
+      <c r="B33">
+        <v>100</v>
+      </c>
+      <c r="C33">
+        <v>100</v>
+      </c>
+      <c r="D33">
+        <v>100</v>
+      </c>
+      <c r="E33">
+        <v>10000</v>
+      </c>
+      <c r="F33">
+        <v>10000</v>
+      </c>
+      <c r="G33">
+        <v>10000</v>
+      </c>
+      <c r="H33">
+        <v>50000</v>
+      </c>
+      <c r="I33">
+        <v>50000</v>
+      </c>
+      <c r="J33">
+        <v>50000</v>
+      </c>
+      <c r="K33">
+        <v>50000</v>
+      </c>
+      <c r="L33">
+        <v>200000</v>
+      </c>
+      <c r="M33">
+        <v>200000</v>
+      </c>
+      <c r="N33">
+        <v>200000</v>
+      </c>
+      <c r="P33" t="s">
+        <v>6</v>
+      </c>
+      <c r="Q33" t="s">
+        <v>7</v>
+      </c>
+      <c r="R33" t="s">
+        <v>8</v>
+      </c>
+      <c r="S33" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="T33" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="U33" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="V33" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="W33" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="X33" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="Y33" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z33" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="AA33" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="AB33" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="AC33" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="AD33" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="AE33" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="AF33" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="AG33" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="AH33" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="AI33" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="AJ33" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="AK33" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="AL33" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="AM33" t="s">
+        <v>29</v>
+      </c>
+      <c r="AN33" s="2" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="34" spans="2:40">
+      <c r="B34">
+        <v>0</v>
+      </c>
+      <c r="C34">
+        <v>100</v>
+      </c>
+      <c r="D34">
+        <v>10000</v>
+      </c>
+      <c r="E34">
+        <v>0</v>
+      </c>
+      <c r="F34">
+        <v>10000</v>
+      </c>
+      <c r="G34">
+        <v>1000000</v>
+      </c>
+      <c r="H34">
+        <v>0</v>
+      </c>
+      <c r="I34">
+        <v>1000000</v>
+      </c>
+      <c r="J34">
+        <v>50000</v>
+      </c>
+      <c r="K34">
+        <v>5000000</v>
+      </c>
+      <c r="L34">
+        <v>0</v>
+      </c>
+      <c r="M34">
+        <v>200000</v>
+      </c>
+      <c r="N34">
+        <v>2000000</v>
+      </c>
+      <c r="P34">
+        <f>MAX(Q34,Q34+R34)</f>
+        <v>100</v>
+      </c>
+      <c r="Q34">
+        <v>100</v>
+      </c>
+      <c r="R34">
+        <v>0</v>
+      </c>
+      <c r="S34" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="T34" s="2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="U34" s="2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="V34" s="2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="W34" s="2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="X34" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="Y34" s="2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="Z34" s="2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="AA34" s="2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="AB34" s="2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="AC34" s="2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="AD34" s="2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="AE34" s="2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="AF34" s="2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="AG34" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AH34" s="2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="AI34" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AJ34" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AK34" s="2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="AL34" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AN34" s="2">
+        <f>AVERAGE(S34:AL34)</f>
+        <v>4.3000000000000026E-3</v>
+      </c>
+    </row>
+    <row r="35" spans="2:40">
+      <c r="B35" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C35" s="2">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D35" s="2">
+        <v>5.5E-2</v>
+      </c>
+      <c r="E35" s="2">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="F35" s="2">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="G35" s="2">
+        <v>6.6369999999999996</v>
+      </c>
+      <c r="H35" s="2">
+        <v>0.39500000000000002</v>
+      </c>
+      <c r="I35" s="2">
+        <v>9.4849999999999994</v>
+      </c>
+      <c r="J35" s="2">
+        <v>0.85899999999999999</v>
+      </c>
+      <c r="K35" s="2">
+        <v>39.244999999999997</v>
+      </c>
+      <c r="L35" s="2">
+        <v>1.754</v>
+      </c>
+      <c r="M35" s="2">
+        <v>3.1549999999999998</v>
+      </c>
+      <c r="N35" s="2">
+        <v>16.806999999999999</v>
+      </c>
+      <c r="P35">
+        <f>MAX(Q35,Q35+R35)</f>
+        <v>200</v>
+      </c>
+      <c r="Q35">
+        <v>100</v>
+      </c>
+      <c r="R35">
+        <v>100</v>
+      </c>
+      <c r="S35" s="2">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="T35" s="2">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="U35" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="V35" s="2">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="W35" s="2">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="X35" s="2">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="Y35" s="2">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="Z35" s="2">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="AA35" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AB35" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AC35" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AD35" s="2">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="AE35" s="2">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="AF35" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AG35" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AH35" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AI35" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AJ35" s="2">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="AK35" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AL35" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="AN35" s="2">
+        <f>AVERAGE(S35:AL35)</f>
+        <v>5.6000000000000017E-3</v>
+      </c>
+    </row>
+    <row r="36" spans="2:40">
+      <c r="B36" s="2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="C36" s="2">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="D36" s="2">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="E36" s="2">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="F36" s="2">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G36" s="2">
+        <v>6.6829999999999998</v>
+      </c>
+      <c r="H36" s="2">
+        <v>0.41199999999999998</v>
+      </c>
+      <c r="I36" s="2">
+        <v>8.1170000000000009</v>
+      </c>
+      <c r="J36" s="2">
+        <v>0.77300000000000002</v>
+      </c>
+      <c r="K36" s="2">
+        <v>38.661000000000001</v>
+      </c>
+      <c r="L36" s="2">
+        <v>1.6639999999999999</v>
+      </c>
+      <c r="M36" s="2">
+        <v>3.1859999999999999</v>
+      </c>
+      <c r="N36" s="2">
+        <v>16.542999999999999</v>
+      </c>
+      <c r="P36">
+        <f>MAX(Q36,Q36+R36)</f>
+        <v>10000</v>
+      </c>
+      <c r="Q36">
+        <v>10000</v>
+      </c>
+      <c r="R36">
+        <v>0</v>
+      </c>
+      <c r="S36" s="2">
+        <v>7.0999999999999994E-2</v>
+      </c>
+      <c r="T36" s="2">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="U36" s="2">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="V36" s="2">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="W36" s="2">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="X36" s="2">
+        <v>7.8E-2</v>
+      </c>
+      <c r="Y36" s="2">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="Z36" s="2">
+        <v>7.8E-2</v>
+      </c>
+      <c r="AA36" s="2">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="AB36" s="2">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="AC36" s="2">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="AD36" s="2">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="AE36" s="2">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="AF36" s="2">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="AG36" s="2">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="AH36" s="2">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="AI36" s="2">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="AJ36" s="2">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="AK36" s="2">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="AL36" s="2">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="AN36" s="2">
+        <f>AVERAGE(S36:AL36)</f>
+        <v>7.3449999999999988E-2</v>
+      </c>
+    </row>
+    <row r="37" spans="2:40">
+      <c r="B37" s="2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="C37" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D37" s="2">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="E37" s="2">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="F37" s="2">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="G37" s="2">
+        <v>6.67</v>
+      </c>
+      <c r="H37" s="2">
+        <v>0.38</v>
+      </c>
+      <c r="I37" s="2">
+        <v>7.9850000000000003</v>
+      </c>
+      <c r="J37" s="2">
+        <v>0.78300000000000003</v>
+      </c>
+      <c r="K37" s="2">
+        <v>39.603000000000002</v>
+      </c>
+      <c r="L37" s="2">
+        <v>1.653</v>
+      </c>
+      <c r="M37" s="2">
+        <v>3.1680000000000001</v>
+      </c>
+      <c r="N37" s="2">
+        <v>17.158999999999999</v>
+      </c>
+      <c r="P37">
+        <f>MAX(Q37,Q37+R37)</f>
+        <v>10100</v>
+      </c>
+      <c r="Q37">
+        <v>100</v>
+      </c>
+      <c r="R37">
+        <v>10000</v>
+      </c>
+      <c r="S37" s="2">
+        <v>5.5E-2</v>
+      </c>
+      <c r="T37" s="2">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="U37" s="2">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="V37" s="2">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="W37" s="2">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="X37" s="2">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="Y37" s="2">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="Z37" s="2">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="AA37" s="2">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="AB37" s="2">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="AC37" s="2">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="AD37" s="2">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="AE37" s="2">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="AF37" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="AG37" s="2">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="AH37" s="2">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="AI37" s="2">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="AJ37" s="2">
+        <v>6.2E-2</v>
+      </c>
+      <c r="AK37" s="2">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="AL37" s="2">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="AN37" s="2">
+        <f>AVERAGE(S37:AL37)</f>
+        <v>5.7400000000000007E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="2:40">
+      <c r="B38" s="2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="C38" s="2">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D38" s="2">
+        <v>6.8000000000000005E-2</v>
+      </c>
+      <c r="E38" s="2">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="F38" s="2">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="G38" s="2">
+        <v>6.5839999999999996</v>
+      </c>
+      <c r="H38" s="2">
+        <v>0.39900000000000002</v>
+      </c>
+      <c r="I38" s="2">
+        <v>7.9489999999999998</v>
+      </c>
+      <c r="J38" s="2">
+        <v>0.78600000000000003</v>
+      </c>
+      <c r="K38" s="2">
+        <v>39.417000000000002</v>
+      </c>
+      <c r="L38" s="2">
+        <v>1.69</v>
+      </c>
+      <c r="M38" s="2">
+        <v>3.1720000000000002</v>
+      </c>
+      <c r="N38" s="2">
+        <v>16.841999999999999</v>
+      </c>
+      <c r="P38">
+        <f>MAX(Q38,Q38+R38)</f>
+        <v>20000</v>
+      </c>
+      <c r="Q38">
+        <v>10000</v>
+      </c>
+      <c r="R38">
+        <v>10000</v>
+      </c>
+      <c r="S38" s="2">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="T38" s="2">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="U38" s="2">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="V38" s="2">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="W38" s="2">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="X38" s="2">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="Y38" s="2">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="Z38" s="2">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="AA38" s="2">
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="AB38" s="2">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="AC38" s="2">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="AD38" s="2">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="AE38" s="2">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="AF38" s="2">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="AG38" s="2">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="AH38" s="2">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="AI38" s="2">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="AJ38" s="2">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="AK38" s="2">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="AL38" s="2">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="AN38" s="2">
+        <f>AVERAGE(S38:AL38)</f>
+        <v>0.1386</v>
+      </c>
+    </row>
+    <row r="39" spans="2:40">
+      <c r="B39" s="2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="C39" s="2">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D39" s="2">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="E39" s="2">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="F39" s="2">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="G39" s="2">
+        <v>6.6609999999999996</v>
+      </c>
+      <c r="H39" s="2">
+        <v>0.42099999999999999</v>
+      </c>
+      <c r="I39" s="2">
+        <v>8.1069999999999993</v>
+      </c>
+      <c r="J39" s="2">
+        <v>0.78700000000000003</v>
+      </c>
+      <c r="K39" s="2">
+        <v>37.843000000000004</v>
+      </c>
+      <c r="L39" s="2">
+        <v>1.6319999999999999</v>
+      </c>
+      <c r="M39" s="2">
+        <v>3.1909999999999998</v>
+      </c>
+      <c r="N39" s="2">
+        <v>16.030999999999999</v>
+      </c>
+      <c r="P39">
+        <f>MAX(Q39,Q39+R39)</f>
+        <v>50000</v>
+      </c>
+      <c r="Q39">
+        <v>50000</v>
+      </c>
+      <c r="R39">
+        <v>0</v>
+      </c>
+      <c r="S39" s="2">
+        <v>0.39500000000000002</v>
+      </c>
+      <c r="T39" s="2">
+        <v>0.41199999999999998</v>
+      </c>
+      <c r="U39" s="2">
+        <v>0.38</v>
+      </c>
+      <c r="V39" s="2">
+        <v>0.39900000000000002</v>
+      </c>
+      <c r="W39" s="2">
+        <v>0.42099999999999999</v>
+      </c>
+      <c r="X39" s="2">
+        <v>0.378</v>
+      </c>
+      <c r="Y39" s="2">
+        <v>0.39200000000000002</v>
+      </c>
+      <c r="Z39" s="2">
+        <v>0.40300000000000002</v>
+      </c>
+      <c r="AA39" s="2">
+        <v>0.40100000000000002</v>
+      </c>
+      <c r="AB39" s="2">
+        <v>0.40699999999999997</v>
+      </c>
+      <c r="AC39" s="2">
+        <v>0.40699999999999997</v>
+      </c>
+      <c r="AD39" s="2">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="AE39" s="2">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="AF39" s="2">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="AG39" s="2">
+        <v>0.39600000000000002</v>
+      </c>
+      <c r="AH39" s="2">
+        <v>0.39700000000000002</v>
+      </c>
+      <c r="AI39" s="2">
+        <v>0.42199999999999999</v>
+      </c>
+      <c r="AJ39" s="2">
+        <v>0.40899999999999997</v>
+      </c>
+      <c r="AK39" s="2">
+        <v>0.39900000000000002</v>
+      </c>
+      <c r="AL39" s="2">
+        <v>0.43</v>
+      </c>
+      <c r="AN39" s="2">
+        <f>AVERAGE(S39:AL39)</f>
+        <v>0.40014999999999989</v>
+      </c>
+    </row>
+    <row r="40" spans="2:40">
+      <c r="B40" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C40" s="2">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D40" s="2">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="E40" s="2">
+        <v>7.8E-2</v>
+      </c>
+      <c r="F40" s="2">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="G40" s="2">
+        <v>7.0609999999999999</v>
+      </c>
+      <c r="H40" s="2">
+        <v>0.378</v>
+      </c>
+      <c r="I40" s="2">
+        <v>8.2919999999999998</v>
+      </c>
+      <c r="J40" s="2">
+        <v>0.80700000000000005</v>
+      </c>
+      <c r="K40" s="2">
+        <v>37.598999999999997</v>
+      </c>
+      <c r="L40" s="2">
+        <v>1.571</v>
+      </c>
+      <c r="M40" s="2">
+        <v>3.2450000000000001</v>
+      </c>
+      <c r="N40" s="2">
+        <v>16.314</v>
+      </c>
+      <c r="P40">
+        <f>MAX(Q40,Q40+R40)</f>
+        <v>100000</v>
+      </c>
+      <c r="Q40">
+        <v>50000</v>
+      </c>
+      <c r="R40">
+        <v>50000</v>
+      </c>
+      <c r="S40" s="2">
+        <v>0.85899999999999999</v>
+      </c>
+      <c r="T40" s="2">
+        <v>0.77300000000000002</v>
+      </c>
+      <c r="U40" s="2">
+        <v>0.78300000000000003</v>
+      </c>
+      <c r="V40" s="2">
+        <v>0.78600000000000003</v>
+      </c>
+      <c r="W40" s="2">
+        <v>0.78700000000000003</v>
+      </c>
+      <c r="X40" s="2">
+        <v>0.80700000000000005</v>
+      </c>
+      <c r="Y40" s="2">
+        <v>0.75800000000000001</v>
+      </c>
+      <c r="Z40" s="2">
+        <v>0.75700000000000001</v>
+      </c>
+      <c r="AA40" s="2">
+        <v>0.77900000000000003</v>
+      </c>
+      <c r="AB40" s="2">
+        <v>0.75900000000000001</v>
+      </c>
+      <c r="AC40" s="2">
+        <v>0.77100000000000002</v>
+      </c>
+      <c r="AD40" s="2">
+        <v>0.77</v>
+      </c>
+      <c r="AE40" s="2">
+        <v>0.75900000000000001</v>
+      </c>
+      <c r="AF40" s="2">
+        <v>0.77</v>
+      </c>
+      <c r="AG40" s="2">
+        <v>0.76</v>
+      </c>
+      <c r="AH40" s="2">
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="AI40" s="2">
+        <v>0.73699999999999999</v>
+      </c>
+      <c r="AJ40" s="2">
+        <v>0.77300000000000002</v>
+      </c>
+      <c r="AK40" s="2">
+        <v>0.78400000000000003</v>
+      </c>
+      <c r="AL40" s="2">
+        <v>0.77600000000000002</v>
+      </c>
+      <c r="AN40" s="2">
+        <f>AVERAGE(S40:AL40)</f>
+        <v>0.77549999999999997</v>
+      </c>
+    </row>
+    <row r="41" spans="2:40">
+      <c r="B41" s="2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="C41" s="2">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D41" s="2">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="E41" s="2">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="F41" s="2">
+        <v>0.13100000000000001</v>
+      </c>
+      <c r="G41" s="2">
+        <v>6.62</v>
+      </c>
+      <c r="H41" s="2">
+        <v>0.39200000000000002</v>
+      </c>
+      <c r="I41" s="2">
+        <v>7.9080000000000004</v>
+      </c>
+      <c r="J41" s="2">
+        <v>0.75800000000000001</v>
+      </c>
+      <c r="K41" s="2">
+        <v>39.250999999999998</v>
+      </c>
+      <c r="L41" s="2">
+        <v>1.585</v>
+      </c>
+      <c r="M41" s="2">
+        <v>3.1989999999999998</v>
+      </c>
+      <c r="N41" s="2">
+        <v>16.882000000000001</v>
+      </c>
+      <c r="P41">
+        <f>MAX(Q41,Q41+R41)</f>
+        <v>200000</v>
+      </c>
+      <c r="Q41">
+        <v>200000</v>
+      </c>
+      <c r="R41">
+        <v>0</v>
+      </c>
+      <c r="S41" s="2">
+        <v>1.754</v>
+      </c>
+      <c r="T41" s="2">
+        <v>1.6639999999999999</v>
+      </c>
+      <c r="U41" s="2">
+        <v>1.653</v>
+      </c>
+      <c r="V41" s="2">
+        <v>1.69</v>
+      </c>
+      <c r="W41" s="2">
+        <v>1.6319999999999999</v>
+      </c>
+      <c r="X41" s="2">
+        <v>1.571</v>
+      </c>
+      <c r="Y41" s="2">
+        <v>1.585</v>
+      </c>
+      <c r="Z41" s="2">
+        <v>1.5860000000000001</v>
+      </c>
+      <c r="AA41" s="2">
+        <v>1.617</v>
+      </c>
+      <c r="AB41" s="2">
+        <v>1.6080000000000001</v>
+      </c>
+      <c r="AC41" s="2">
+        <v>1.611</v>
+      </c>
+      <c r="AD41" s="2">
+        <v>1.617</v>
+      </c>
+      <c r="AE41" s="2">
+        <v>1.63</v>
+      </c>
+      <c r="AF41" s="2">
+        <v>1.5720000000000001</v>
+      </c>
+      <c r="AG41" s="2">
+        <v>1.5720000000000001</v>
+      </c>
+      <c r="AH41" s="2">
+        <v>1.5760000000000001</v>
+      </c>
+      <c r="AI41" s="2">
+        <v>1.595</v>
+      </c>
+      <c r="AJ41" s="2">
+        <v>1.5760000000000001</v>
+      </c>
+      <c r="AK41" s="2">
+        <v>1.595</v>
+      </c>
+      <c r="AL41" s="2">
+        <v>1.625</v>
+      </c>
+      <c r="AN41" s="2">
+        <f>AVERAGE(S41:AL41)</f>
+        <v>1.6164499999999997</v>
+      </c>
+    </row>
+    <row r="42" spans="2:40">
+      <c r="B42" s="2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="C42" s="2">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="D42" s="2">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="E42" s="2">
+        <v>7.8E-2</v>
+      </c>
+      <c r="F42" s="2">
+        <v>0.13600000000000001</v>
+      </c>
+      <c r="G42" s="2">
+        <v>6.6630000000000003</v>
+      </c>
+      <c r="H42" s="2">
+        <v>0.40300000000000002</v>
+      </c>
+      <c r="I42" s="2">
+        <v>7.9489999999999998</v>
+      </c>
+      <c r="J42" s="2">
+        <v>0.75700000000000001</v>
+      </c>
+      <c r="K42" s="2">
+        <v>37.289000000000001</v>
+      </c>
+      <c r="L42" s="2">
+        <v>1.5860000000000001</v>
+      </c>
+      <c r="M42" s="2">
+        <v>3.1480000000000001</v>
+      </c>
+      <c r="N42" s="2">
+        <v>16.847999999999999</v>
+      </c>
+      <c r="P42">
+        <f>MAX(Q42,Q42+R42)</f>
+        <v>400000</v>
+      </c>
+      <c r="Q42">
+        <v>200000</v>
+      </c>
+      <c r="R42">
+        <v>200000</v>
+      </c>
+      <c r="S42" s="2">
+        <v>3.1549999999999998</v>
+      </c>
+      <c r="T42" s="2">
+        <v>3.1859999999999999</v>
+      </c>
+      <c r="U42" s="2">
+        <v>3.1680000000000001</v>
+      </c>
+      <c r="V42" s="2">
+        <v>3.1720000000000002</v>
+      </c>
+      <c r="W42" s="2">
+        <v>3.1909999999999998</v>
+      </c>
+      <c r="X42" s="2">
+        <v>3.2450000000000001</v>
+      </c>
+      <c r="Y42" s="2">
+        <v>3.1989999999999998</v>
+      </c>
+      <c r="Z42" s="2">
+        <v>3.1480000000000001</v>
+      </c>
+      <c r="AA42" s="2">
+        <v>3.0950000000000002</v>
+      </c>
+      <c r="AB42" s="2">
+        <v>3.1339999999999999</v>
+      </c>
+      <c r="AC42" s="2">
+        <v>3.2509999999999999</v>
+      </c>
+      <c r="AD42" s="2">
+        <v>3.11</v>
+      </c>
+      <c r="AE42" s="2">
+        <v>3.2440000000000002</v>
+      </c>
+      <c r="AF42" s="2">
+        <v>3.3260000000000001</v>
+      </c>
+      <c r="AG42" s="2">
+        <v>3.3919999999999999</v>
+      </c>
+      <c r="AH42" s="2">
+        <v>3.2130000000000001</v>
+      </c>
+      <c r="AI42" s="2">
+        <v>3.2040000000000002</v>
+      </c>
+      <c r="AJ42" s="2">
+        <v>3.13</v>
+      </c>
+      <c r="AK42" s="2">
+        <v>3.141</v>
+      </c>
+      <c r="AL42" s="2">
+        <v>3.1640000000000001</v>
+      </c>
+      <c r="AN42" s="2">
+        <f>AVERAGE(S42:AL42)</f>
+        <v>3.1934000000000005</v>
+      </c>
+    </row>
+    <row r="43" spans="2:40">
+      <c r="B43" s="2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="C43" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D43" s="2">
+        <v>5.1999999999999998E-2</v>
+      </c>
+      <c r="E43" s="2">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="F43" s="2">
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="G43" s="2">
+        <v>6.8019999999999996</v>
+      </c>
+      <c r="H43" s="2">
+        <v>0.40100000000000002</v>
+      </c>
+      <c r="I43" s="2">
+        <v>7.9969999999999999</v>
+      </c>
+      <c r="J43" s="2">
+        <v>0.77900000000000003</v>
+      </c>
+      <c r="K43" s="2">
+        <v>39.225999999999999</v>
+      </c>
+      <c r="L43" s="2">
+        <v>1.617</v>
+      </c>
+      <c r="M43" s="2">
+        <v>3.0950000000000002</v>
+      </c>
+      <c r="N43" s="2">
+        <v>16.116</v>
+      </c>
+      <c r="P43">
+        <f>MAX(Q43,Q43+R43)</f>
+        <v>1010000</v>
+      </c>
+      <c r="Q43">
+        <v>10000</v>
+      </c>
+      <c r="R43">
+        <v>1000000</v>
+      </c>
+      <c r="S43" s="2">
+        <v>6.6369999999999996</v>
+      </c>
+      <c r="T43" s="2">
+        <v>6.6829999999999998</v>
+      </c>
+      <c r="U43" s="2">
+        <v>6.67</v>
+      </c>
+      <c r="V43" s="2">
+        <v>6.5839999999999996</v>
+      </c>
+      <c r="W43" s="2">
+        <v>6.6609999999999996</v>
+      </c>
+      <c r="X43" s="2">
+        <v>7.0609999999999999</v>
+      </c>
+      <c r="Y43" s="2">
+        <v>6.62</v>
+      </c>
+      <c r="Z43" s="2">
+        <v>6.6630000000000003</v>
+      </c>
+      <c r="AA43" s="2">
+        <v>6.8019999999999996</v>
+      </c>
+      <c r="AB43" s="2">
+        <v>6.5640000000000001</v>
+      </c>
+      <c r="AC43" s="2">
+        <v>6.6050000000000004</v>
+      </c>
+      <c r="AD43" s="2">
+        <v>6.6379999999999999</v>
+      </c>
+      <c r="AE43" s="2">
+        <v>6.6749999999999998</v>
+      </c>
+      <c r="AF43" s="2">
+        <v>6.7629999999999999</v>
+      </c>
+      <c r="AG43" s="2">
+        <v>6.7290000000000001</v>
+      </c>
+      <c r="AH43" s="2">
+        <v>6.6390000000000002</v>
+      </c>
+      <c r="AI43" s="2">
+        <v>6.6340000000000003</v>
+      </c>
+      <c r="AJ43" s="2">
+        <v>6.6879999999999997</v>
+      </c>
+      <c r="AK43" s="2">
+        <v>7.6840000000000002</v>
+      </c>
+      <c r="AL43" s="2">
+        <v>7.1029999999999998</v>
+      </c>
+      <c r="AN43" s="2">
+        <f>AVERAGE(S43:AL43)</f>
+        <v>6.7551500000000004</v>
+      </c>
+    </row>
+    <row r="44" spans="2:40">
+      <c r="B44" s="2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="C44" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D44" s="2">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="E44" s="2">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="F44" s="2">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="G44" s="2">
+        <v>6.5640000000000001</v>
+      </c>
+      <c r="H44" s="2">
+        <v>0.40699999999999997</v>
+      </c>
+      <c r="I44" s="2">
+        <v>8.0090000000000003</v>
+      </c>
+      <c r="J44" s="2">
+        <v>0.75900000000000001</v>
+      </c>
+      <c r="K44" s="2">
+        <v>40.521000000000001</v>
+      </c>
+      <c r="L44" s="2">
+        <v>1.6080000000000001</v>
+      </c>
+      <c r="M44" s="2">
+        <v>3.1339999999999999</v>
+      </c>
+      <c r="N44" s="2">
+        <v>15.903</v>
+      </c>
+      <c r="P44">
+        <f>MAX(Q44,Q44+R44)</f>
+        <v>1050000</v>
+      </c>
+      <c r="Q44">
+        <v>50000</v>
+      </c>
+      <c r="R44">
+        <v>1000000</v>
+      </c>
+      <c r="S44" s="2">
+        <v>9.4849999999999994</v>
+      </c>
+      <c r="T44" s="2">
+        <v>8.1170000000000009</v>
+      </c>
+      <c r="U44" s="2">
+        <v>7.9850000000000003</v>
+      </c>
+      <c r="V44" s="2">
+        <v>7.9489999999999998</v>
+      </c>
+      <c r="W44" s="2">
+        <v>8.1069999999999993</v>
+      </c>
+      <c r="X44" s="2">
+        <v>8.2919999999999998</v>
+      </c>
+      <c r="Y44" s="2">
+        <v>7.9080000000000004</v>
+      </c>
+      <c r="Z44" s="2">
+        <v>7.9489999999999998</v>
+      </c>
+      <c r="AA44" s="2">
+        <v>7.9969999999999999</v>
+      </c>
+      <c r="AB44" s="2">
+        <v>8.0090000000000003</v>
+      </c>
+      <c r="AC44" s="2">
+        <v>7.8579999999999997</v>
+      </c>
+      <c r="AD44" s="2">
+        <v>7.9889999999999999</v>
+      </c>
+      <c r="AE44" s="2">
+        <v>7.7869999999999999</v>
+      </c>
+      <c r="AF44" s="2">
+        <v>8.0129999999999999</v>
+      </c>
+      <c r="AG44" s="2">
+        <v>7.9889999999999999</v>
+      </c>
+      <c r="AH44" s="2">
+        <v>8.0289999999999999</v>
+      </c>
+      <c r="AI44" s="2">
+        <v>7.8540000000000001</v>
+      </c>
+      <c r="AJ44" s="2">
+        <v>7.8639999999999999</v>
+      </c>
+      <c r="AK44" s="2">
+        <v>7.984</v>
+      </c>
+      <c r="AL44" s="2">
+        <v>8.0220000000000002</v>
+      </c>
+      <c r="AN44" s="2">
+        <f>AVERAGE(S44:AL44)</f>
+        <v>8.059350000000002</v>
+      </c>
+    </row>
+    <row r="45" spans="2:40">
+      <c r="B45" s="2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="C45" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D45" s="2">
+        <v>5.3999999999999999E-2</v>
+      </c>
+      <c r="E45" s="2">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="F45" s="2">
+        <v>0.14399999999999999</v>
+      </c>
+      <c r="G45" s="2">
+        <v>6.6050000000000004</v>
+      </c>
+      <c r="H45" s="2">
+        <v>0.40699999999999997</v>
+      </c>
+      <c r="I45" s="2">
+        <v>7.8579999999999997</v>
+      </c>
+      <c r="J45" s="2">
+        <v>0.77100000000000002</v>
+      </c>
+      <c r="K45" s="2">
+        <v>42.136000000000003</v>
+      </c>
+      <c r="L45" s="2">
+        <v>1.611</v>
+      </c>
+      <c r="M45" s="2">
+        <v>3.2509999999999999</v>
+      </c>
+      <c r="N45" s="2">
+        <v>16.742000000000001</v>
+      </c>
+      <c r="P45">
+        <f>MAX(Q45,Q45+R45)</f>
+        <v>2200000</v>
+      </c>
+      <c r="Q45">
+        <v>200000</v>
+      </c>
+      <c r="R45">
+        <v>2000000</v>
+      </c>
+      <c r="S45" s="2">
+        <v>16.806999999999999</v>
+      </c>
+      <c r="T45" s="2">
+        <v>16.542999999999999</v>
+      </c>
+      <c r="U45" s="2">
+        <v>17.158999999999999</v>
+      </c>
+      <c r="V45" s="2">
+        <v>16.841999999999999</v>
+      </c>
+      <c r="W45" s="2">
+        <v>16.030999999999999</v>
+      </c>
+      <c r="X45" s="2">
+        <v>16.314</v>
+      </c>
+      <c r="Y45" s="2">
+        <v>16.882000000000001</v>
+      </c>
+      <c r="Z45" s="2">
+        <v>16.847999999999999</v>
+      </c>
+      <c r="AA45" s="2">
+        <v>16.116</v>
+      </c>
+      <c r="AB45" s="2">
+        <v>15.903</v>
+      </c>
+      <c r="AC45" s="2">
+        <v>16.742000000000001</v>
+      </c>
+      <c r="AD45" s="2">
+        <v>16.798999999999999</v>
+      </c>
+      <c r="AE45" s="2">
+        <v>16.844000000000001</v>
+      </c>
+      <c r="AF45" s="2">
+        <v>16.228999999999999</v>
+      </c>
+      <c r="AG45" s="2">
+        <v>16.699000000000002</v>
+      </c>
+      <c r="AH45" s="2">
+        <v>16.486999999999998</v>
+      </c>
+      <c r="AI45" s="2">
+        <v>15.925000000000001</v>
+      </c>
+      <c r="AJ45" s="2">
+        <v>16.36</v>
+      </c>
+      <c r="AK45" s="2">
+        <v>18.38</v>
+      </c>
+      <c r="AL45" s="2">
+        <v>17.611000000000001</v>
+      </c>
+      <c r="AN45" s="2">
+        <f>AVERAGE(S45:AL45)</f>
+        <v>16.67605</v>
+      </c>
+    </row>
+    <row r="46" spans="2:40">
+      <c r="B46" s="2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="C46" s="2">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D46" s="2">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="E46" s="2">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="F46" s="2">
+        <v>0.13500000000000001</v>
+      </c>
+      <c r="G46" s="2">
+        <v>6.6379999999999999</v>
+      </c>
+      <c r="H46" s="2">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="I46" s="2">
+        <v>7.9889999999999999</v>
+      </c>
+      <c r="J46" s="2">
+        <v>0.77</v>
+      </c>
+      <c r="K46" s="2">
+        <v>39.906999999999996</v>
+      </c>
+      <c r="L46" s="2">
+        <v>1.617</v>
+      </c>
+      <c r="M46" s="2">
+        <v>3.11</v>
+      </c>
+      <c r="N46" s="2">
+        <v>16.798999999999999</v>
+      </c>
+      <c r="P46">
+        <f>MAX(Q46,Q46+R46)</f>
+        <v>5050000</v>
+      </c>
+      <c r="Q46">
+        <v>50000</v>
+      </c>
+      <c r="R46">
+        <v>5000000</v>
+      </c>
+      <c r="S46" s="2">
+        <v>39.244999999999997</v>
+      </c>
+      <c r="T46" s="2">
+        <v>38.661000000000001</v>
+      </c>
+      <c r="U46" s="2">
+        <v>39.603000000000002</v>
+      </c>
+      <c r="V46" s="2">
+        <v>39.417000000000002</v>
+      </c>
+      <c r="W46" s="2">
+        <v>37.843000000000004</v>
+      </c>
+      <c r="X46" s="2">
+        <v>37.598999999999997</v>
+      </c>
+      <c r="Y46" s="2">
+        <v>39.250999999999998</v>
+      </c>
+      <c r="Z46" s="2">
+        <v>37.289000000000001</v>
+      </c>
+      <c r="AA46" s="2">
+        <v>39.225999999999999</v>
+      </c>
+      <c r="AB46" s="2">
+        <v>40.521000000000001</v>
+      </c>
+      <c r="AC46" s="2">
+        <v>42.136000000000003</v>
+      </c>
+      <c r="AD46" s="2">
+        <v>39.906999999999996</v>
+      </c>
+      <c r="AE46" s="2">
+        <v>38.389000000000003</v>
+      </c>
+      <c r="AF46" s="2">
+        <v>35.938000000000002</v>
+      </c>
+      <c r="AG46" s="2">
+        <v>40.164999999999999</v>
+      </c>
+      <c r="AH46" s="2">
+        <v>40.201999999999998</v>
+      </c>
+      <c r="AI46" s="2">
+        <v>40.042000000000002</v>
+      </c>
+      <c r="AJ46" s="2">
+        <v>46.317</v>
+      </c>
+      <c r="AK46" s="2">
+        <v>41.621000000000002</v>
+      </c>
+      <c r="AL46" s="2">
+        <v>37.539000000000001</v>
+      </c>
+      <c r="AN46" s="2">
+        <f>AVERAGE(S46:AL46)</f>
+        <v>39.545549999999999</v>
+      </c>
+    </row>
+    <row r="47" spans="2:40">
+      <c r="B47" s="2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="C47" s="2">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D47" s="2">
+        <v>6.0999999999999999E-2</v>
+      </c>
+      <c r="E47" s="2">
+        <v>7.5999999999999998E-2</v>
+      </c>
+      <c r="F47" s="2">
+        <v>0.14199999999999999</v>
+      </c>
+      <c r="G47" s="2">
+        <v>6.6749999999999998</v>
+      </c>
+      <c r="H47" s="2">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="I47" s="2">
+        <v>7.7869999999999999</v>
+      </c>
+      <c r="J47" s="2">
+        <v>0.75900000000000001</v>
+      </c>
+      <c r="K47" s="2">
+        <v>38.389000000000003</v>
+      </c>
+      <c r="L47" s="2">
+        <v>1.63</v>
+      </c>
+      <c r="M47" s="2">
+        <v>3.2440000000000002</v>
+      </c>
+      <c r="N47" s="2">
+        <v>16.844000000000001</v>
+      </c>
+    </row>
+    <row r="48" spans="2:40">
+      <c r="B48" s="2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="C48" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D48" s="2">
+        <v>7.0000000000000007E-2</v>
+      </c>
+      <c r="E48" s="2">
+        <v>7.3999999999999996E-2</v>
+      </c>
+      <c r="F48" s="2">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G48" s="2">
+        <v>6.7629999999999999</v>
+      </c>
+      <c r="H48" s="2">
+        <v>0.38500000000000001</v>
+      </c>
+      <c r="I48" s="2">
+        <v>8.0129999999999999</v>
+      </c>
+      <c r="J48" s="2">
+        <v>0.77</v>
+      </c>
+      <c r="K48" s="2">
+        <v>35.938000000000002</v>
+      </c>
+      <c r="L48" s="2">
+        <v>1.5720000000000001</v>
+      </c>
+      <c r="M48" s="2">
+        <v>3.3260000000000001</v>
+      </c>
+      <c r="N48" s="2">
+        <v>16.228999999999999</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14">
+      <c r="B49" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C49" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D49" s="2">
+        <v>6.5000000000000002E-2</v>
+      </c>
+      <c r="E49" s="2">
+        <v>7.2999999999999995E-2</v>
+      </c>
+      <c r="F49" s="2">
+        <v>0.13300000000000001</v>
+      </c>
+      <c r="G49" s="2">
+        <v>6.7290000000000001</v>
+      </c>
+      <c r="H49" s="2">
+        <v>0.39600000000000002</v>
+      </c>
+      <c r="I49" s="2">
+        <v>7.9889999999999999</v>
+      </c>
+      <c r="J49" s="2">
+        <v>0.76</v>
+      </c>
+      <c r="K49" s="2">
+        <v>40.164999999999999</v>
+      </c>
+      <c r="L49" s="2">
+        <v>1.5720000000000001</v>
+      </c>
+      <c r="M49" s="2">
+        <v>3.3919999999999999</v>
+      </c>
+      <c r="N49" s="2">
+        <v>16.699000000000002</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14">
+      <c r="B50" s="2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="C50" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D50" s="2">
+        <v>5.8000000000000003E-2</v>
+      </c>
+      <c r="E50" s="2">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="F50" s="2">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G50" s="2">
+        <v>6.6390000000000002</v>
+      </c>
+      <c r="H50" s="2">
+        <v>0.39700000000000002</v>
+      </c>
+      <c r="I50" s="2">
+        <v>8.0289999999999999</v>
+      </c>
+      <c r="J50" s="2">
+        <v>0.76200000000000001</v>
+      </c>
+      <c r="K50" s="2">
+        <v>40.201999999999998</v>
+      </c>
+      <c r="L50" s="2">
+        <v>1.5760000000000001</v>
+      </c>
+      <c r="M50" s="2">
+        <v>3.2130000000000001</v>
+      </c>
+      <c r="N50" s="2">
+        <v>16.486999999999998</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14">
+      <c r="B51" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C51" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D51" s="2">
+        <v>5.6000000000000001E-2</v>
+      </c>
+      <c r="E51" s="2">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="F51" s="2">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="G51" s="2">
+        <v>6.6340000000000003</v>
+      </c>
+      <c r="H51" s="2">
+        <v>0.42199999999999999</v>
+      </c>
+      <c r="I51" s="2">
+        <v>7.8540000000000001</v>
+      </c>
+      <c r="J51" s="2">
+        <v>0.73699999999999999</v>
+      </c>
+      <c r="K51" s="2">
+        <v>40.042000000000002</v>
+      </c>
+      <c r="L51" s="2">
+        <v>1.595</v>
+      </c>
+      <c r="M51" s="2">
+        <v>3.2040000000000002</v>
+      </c>
+      <c r="N51" s="2">
+        <v>15.925000000000001</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14">
+      <c r="B52" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C52" s="2">
+        <v>6.0000000000000001E-3</v>
+      </c>
+      <c r="D52" s="2">
+        <v>6.2E-2</v>
+      </c>
+      <c r="E52" s="2">
+        <v>7.1999999999999995E-2</v>
+      </c>
+      <c r="F52" s="2">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="G52" s="2">
+        <v>6.6879999999999997</v>
+      </c>
+      <c r="H52" s="2">
+        <v>0.40899999999999997</v>
+      </c>
+      <c r="I52" s="2">
+        <v>7.8639999999999999</v>
+      </c>
+      <c r="J52" s="2">
+        <v>0.77300000000000002</v>
+      </c>
+      <c r="K52" s="2">
+        <v>46.317</v>
+      </c>
+      <c r="L52" s="2">
+        <v>1.5760000000000001</v>
+      </c>
+      <c r="M52" s="2">
+        <v>3.13</v>
+      </c>
+      <c r="N52" s="2">
+        <v>16.36</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14">
+      <c r="B53" s="2">
+        <v>4.0000000000000001E-3</v>
+      </c>
+      <c r="C53" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D53" s="2">
+        <v>5.2999999999999999E-2</v>
+      </c>
+      <c r="E53" s="2">
+        <v>6.9000000000000006E-2</v>
+      </c>
+      <c r="F53" s="2">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="G53" s="2">
+        <v>7.6840000000000002</v>
+      </c>
+      <c r="H53" s="2">
+        <v>0.39900000000000002</v>
+      </c>
+      <c r="I53" s="2">
+        <v>7.984</v>
+      </c>
+      <c r="J53" s="2">
+        <v>0.78400000000000003</v>
+      </c>
+      <c r="K53" s="2">
+        <v>41.621000000000002</v>
+      </c>
+      <c r="L53" s="2">
+        <v>1.595</v>
+      </c>
+      <c r="M53" s="2">
+        <v>3.141</v>
+      </c>
+      <c r="N53" s="2">
+        <v>18.38</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14">
+      <c r="B54" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="C54" s="2">
+        <v>5.0000000000000001E-3</v>
+      </c>
+      <c r="D54" s="2">
+        <v>5.8999999999999997E-2</v>
+      </c>
+      <c r="E54" s="2">
+        <v>7.4999999999999997E-2</v>
+      </c>
+      <c r="F54" s="2">
+        <v>0.13400000000000001</v>
+      </c>
+      <c r="G54" s="2">
+        <v>7.1029999999999998</v>
+      </c>
+      <c r="H54" s="2">
+        <v>0.43</v>
+      </c>
+      <c r="I54" s="2">
+        <v>8.0220000000000002</v>
+      </c>
+      <c r="J54" s="2">
+        <v>0.77600000000000002</v>
+      </c>
+      <c r="K54" s="2">
+        <v>37.539000000000001</v>
+      </c>
+      <c r="L54" s="2">
+        <v>1.625</v>
+      </c>
+      <c r="M54" s="2">
+        <v>3.1640000000000001</v>
+      </c>
+      <c r="N54" s="2">
+        <v>17.611000000000001</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14">
+      <c r="A56" t="s">
+        <v>4</v>
+      </c>
+      <c r="B56" s="2">
+        <f>AVERAGE(B35:B54)</f>
+        <v>4.3000000000000026E-3</v>
+      </c>
+      <c r="C56" s="2">
+        <f t="shared" ref="C56:N56" si="1">AVERAGE(C35:C54)</f>
+        <v>5.6000000000000017E-3</v>
+      </c>
+      <c r="D56" s="2">
+        <f t="shared" si="1"/>
+        <v>5.7400000000000007E-2</v>
+      </c>
+      <c r="E56" s="2">
+        <f t="shared" si="1"/>
+        <v>7.3449999999999988E-2</v>
+      </c>
+      <c r="F56" s="2">
+        <f t="shared" si="1"/>
+        <v>0.1386</v>
+      </c>
+      <c r="G56" s="2">
+        <f t="shared" si="1"/>
+        <v>6.7551500000000004</v>
+      </c>
+      <c r="H56" s="2">
+        <f t="shared" si="1"/>
+        <v>0.40014999999999989</v>
+      </c>
+      <c r="I56" s="2">
+        <f t="shared" si="1"/>
+        <v>8.059350000000002</v>
+      </c>
+      <c r="J56" s="2">
+        <f t="shared" si="1"/>
+        <v>0.77549999999999997</v>
+      </c>
+      <c r="K56" s="2">
+        <f t="shared" si="1"/>
+        <v>39.545549999999999</v>
+      </c>
+      <c r="L56" s="2">
+        <f t="shared" si="1"/>
+        <v>1.6164499999999997</v>
+      </c>
+      <c r="M56" s="2">
+        <f t="shared" si="1"/>
+        <v>3.1934000000000005</v>
+      </c>
+      <c r="N56" s="2">
+        <f t="shared" si="1"/>
+        <v>16.67605</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="0" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
+  <drawing r:id="rId1"/>
+  <tableParts count="1">
+    <tablePart r:id="rId2"/>
+  </tableParts>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>